<commit_message>
small update to excel
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form_Pedestro.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form_Pedestro.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EEF1CF-D4DB-4CAD-97C9-7C06C79ED274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD39F3F-ADD2-46F6-9E21-59AF0187EDBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="690" windowWidth="28800" windowHeight="15885" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -1487,204 +1487,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1694,23 +1496,221 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2036,12 +2036,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="62"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="71"/>
       <c r="H1" s="35" t="s">
         <v>1</v>
       </c>
@@ -2049,11 +2049,11 @@
       <c r="J1" s="35"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H2" s="63" t="s">
+      <c r="H2" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H3" s="2"/>
@@ -2204,21 +2204,21 @@
     </row>
     <row r="24" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="32"/>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="59"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="68"/>
+      <c r="N24" s="68"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C26" s="34"/>
@@ -2263,12 +2263,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="3" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B3" s="48" t="s">
@@ -2281,37 +2281,37 @@
       <c r="G3" s="50"/>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="G5" s="86" t="s">
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="G5" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="86"/>
-      <c r="L5" s="86"/>
-      <c r="M5" s="86"/>
-      <c r="N5" s="86"/>
-      <c r="O5" s="86"/>
-      <c r="P5" s="86"/>
-      <c r="S5" s="72"/>
-      <c r="T5" s="73"/>
-      <c r="U5" s="73"/>
-      <c r="V5" s="73"/>
-      <c r="W5" s="73"/>
-      <c r="X5" s="73"/>
-      <c r="Y5" s="73"/>
-      <c r="Z5" s="73"/>
-      <c r="AA5" s="73"/>
-      <c r="AB5" s="73"/>
-      <c r="AC5" s="73"/>
-      <c r="AD5" s="73"/>
-      <c r="AE5" s="74"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="84"/>
+      <c r="S5" s="95"/>
+      <c r="T5" s="96"/>
+      <c r="U5" s="96"/>
+      <c r="V5" s="96"/>
+      <c r="W5" s="96"/>
+      <c r="X5" s="96"/>
+      <c r="Y5" s="96"/>
+      <c r="Z5" s="96"/>
+      <c r="AA5" s="96"/>
+      <c r="AB5" s="96"/>
+      <c r="AC5" s="96"/>
+      <c r="AD5" s="96"/>
+      <c r="AE5" s="97"/>
     </row>
     <row r="6" spans="2:31" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
@@ -2326,51 +2326,51 @@
       <c r="E6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="75" t="s">
+      <c r="G6" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="77" t="s">
+      <c r="H6" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="79" t="s">
+      <c r="I6" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="80"/>
-      <c r="M6" s="80"/>
-      <c r="N6" s="80"/>
-      <c r="O6" s="80"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="87"/>
       <c r="P6" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="S6" s="75"/>
-      <c r="T6" s="75"/>
-      <c r="U6" s="75"/>
-      <c r="V6" s="77"/>
-      <c r="W6" s="79"/>
-      <c r="X6" s="80"/>
-      <c r="Y6" s="80"/>
-      <c r="Z6" s="80"/>
-      <c r="AA6" s="80"/>
-      <c r="AB6" s="80"/>
-      <c r="AC6" s="80"/>
-      <c r="AD6" s="81"/>
+      <c r="S6" s="85"/>
+      <c r="T6" s="85"/>
+      <c r="U6" s="85"/>
+      <c r="V6" s="88"/>
+      <c r="W6" s="82"/>
+      <c r="X6" s="87"/>
+      <c r="Y6" s="87"/>
+      <c r="Z6" s="87"/>
+      <c r="AA6" s="87"/>
+      <c r="AB6" s="87"/>
+      <c r="AC6" s="87"/>
+      <c r="AD6" s="83"/>
       <c r="AE6" s="51"/>
     </row>
     <row r="7" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="82" t="s">
+      <c r="C7" s="92" t="s">
         <v>81</v>
       </c>
       <c r="D7" s="47" t="s">
         <v>60</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="78"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="89"/>
       <c r="I7" s="13" t="s">
         <v>62</v>
       </c>
@@ -2386,24 +2386,24 @@
       <c r="M7" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="N7" s="79" t="s">
+      <c r="N7" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="O7" s="81"/>
+      <c r="O7" s="83"/>
       <c r="P7" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="S7" s="76"/>
-      <c r="T7" s="76"/>
-      <c r="U7" s="76"/>
-      <c r="V7" s="78"/>
+      <c r="S7" s="86"/>
+      <c r="T7" s="86"/>
+      <c r="U7" s="86"/>
+      <c r="V7" s="89"/>
       <c r="W7" s="13"/>
       <c r="X7" s="13"/>
       <c r="Y7" s="13"/>
       <c r="Z7" s="13"/>
       <c r="AA7" s="13"/>
-      <c r="AB7" s="79"/>
-      <c r="AC7" s="81"/>
+      <c r="AB7" s="82"/>
+      <c r="AC7" s="83"/>
       <c r="AD7" s="52"/>
       <c r="AE7" s="51"/>
     </row>
@@ -2411,7 +2411,7 @@
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="82"/>
+      <c r="C8" s="92"/>
       <c r="D8" s="4"/>
       <c r="E8" s="46" t="s">
         <v>82</v>
@@ -2419,7 +2419,7 @@
       <c r="G8" s="13">
         <v>1</v>
       </c>
-      <c r="H8" s="126" t="s">
+      <c r="H8" s="60" t="s">
         <v>69</v>
       </c>
       <c r="I8" s="21" t="s">
@@ -2437,10 +2437,10 @@
       <c r="M8" s="21">
         <v>10</v>
       </c>
-      <c r="N8" s="129" t="s">
+      <c r="N8" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="O8" s="130" t="s">
+      <c r="O8" s="81" t="s">
         <v>32</v>
       </c>
       <c r="P8" s="56" t="s">
@@ -2455,8 +2455,8 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
-      <c r="AB8" s="64"/>
-      <c r="AC8" s="65"/>
+      <c r="AB8" s="74"/>
+      <c r="AC8" s="75"/>
       <c r="AD8" s="2"/>
       <c r="AE8" s="50"/>
     </row>
@@ -2464,7 +2464,7 @@
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="83" t="s">
+      <c r="C9" s="90" t="s">
         <v>83</v>
       </c>
       <c r="D9" s="47" t="s">
@@ -2474,7 +2474,7 @@
       <c r="G9" s="13">
         <v>2</v>
       </c>
-      <c r="H9" s="127" t="s">
+      <c r="H9" s="61" t="s">
         <v>71</v>
       </c>
       <c r="I9" s="21" t="s">
@@ -2492,10 +2492,10 @@
       <c r="M9" s="21">
         <v>10</v>
       </c>
-      <c r="N9" s="129" t="s">
+      <c r="N9" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="O9" s="130" t="s">
+      <c r="O9" s="81" t="s">
         <v>32</v>
       </c>
       <c r="P9" s="56" t="s">
@@ -2510,8 +2510,8 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
-      <c r="AB9" s="64"/>
-      <c r="AC9" s="65"/>
+      <c r="AB9" s="74"/>
+      <c r="AC9" s="75"/>
       <c r="AD9" s="2"/>
       <c r="AE9" s="50"/>
     </row>
@@ -2519,7 +2519,7 @@
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="87"/>
+      <c r="C10" s="91"/>
       <c r="D10" s="4"/>
       <c r="E10" s="45" t="s">
         <v>80</v>
@@ -2527,7 +2527,7 @@
       <c r="G10" s="22">
         <v>3</v>
       </c>
-      <c r="H10" s="128" t="s">
+      <c r="H10" s="62" t="s">
         <v>86</v>
       </c>
       <c r="I10" s="21" t="s">
@@ -2545,10 +2545,10 @@
       <c r="M10" s="21">
         <v>10</v>
       </c>
-      <c r="N10" s="129" t="s">
+      <c r="N10" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="O10" s="130" t="s">
+      <c r="O10" s="81" t="s">
         <v>32</v>
       </c>
       <c r="P10" s="56" t="s">
@@ -2563,8 +2563,8 @@
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
       <c r="AA10" s="10"/>
-      <c r="AB10" s="70"/>
-      <c r="AC10" s="71"/>
+      <c r="AB10" s="98"/>
+      <c r="AC10" s="99"/>
       <c r="AD10" s="10"/>
       <c r="AE10" s="56"/>
     </row>
@@ -2574,11 +2574,11 @@
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="125"/>
+      <c r="E11" s="59"/>
       <c r="G11" s="22">
         <v>4</v>
       </c>
-      <c r="H11" s="128" t="s">
+      <c r="H11" s="62" t="s">
         <v>87</v>
       </c>
       <c r="I11" s="21" t="s">
@@ -2596,10 +2596,10 @@
       <c r="M11" s="21">
         <v>10</v>
       </c>
-      <c r="N11" s="129" t="s">
+      <c r="N11" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="O11" s="130" t="s">
+      <c r="O11" s="81" t="s">
         <v>32</v>
       </c>
       <c r="P11" s="56" t="s">
@@ -2614,8 +2614,8 @@
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
       <c r="AA11" s="10"/>
-      <c r="AB11" s="70"/>
-      <c r="AC11" s="71"/>
+      <c r="AB11" s="98"/>
+      <c r="AC11" s="99"/>
       <c r="AD11" s="10"/>
       <c r="AE11" s="53"/>
     </row>
@@ -2635,8 +2635,8 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="67"/>
+      <c r="N12" s="78"/>
+      <c r="O12" s="79"/>
       <c r="P12" s="54"/>
       <c r="S12" s="9"/>
       <c r="T12" s="9"/>
@@ -2647,8 +2647,8 @@
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
-      <c r="AB12" s="66"/>
-      <c r="AC12" s="67"/>
+      <c r="AB12" s="78"/>
+      <c r="AC12" s="79"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="54"/>
     </row>
@@ -2656,7 +2656,7 @@
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="83"/>
+      <c r="C13" s="90"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="G13" s="9">
@@ -2668,8 +2668,8 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
-      <c r="N13" s="66"/>
-      <c r="O13" s="67"/>
+      <c r="N13" s="78"/>
+      <c r="O13" s="79"/>
       <c r="P13" s="54"/>
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
@@ -2680,8 +2680,8 @@
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
       <c r="AA13" s="6"/>
-      <c r="AB13" s="66"/>
-      <c r="AC13" s="67"/>
+      <c r="AB13" s="78"/>
+      <c r="AC13" s="79"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="54"/>
     </row>
@@ -2689,7 +2689,7 @@
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="84"/>
+      <c r="C14" s="93"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="G14" s="12">
@@ -2701,8 +2701,8 @@
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
-      <c r="N14" s="68"/>
-      <c r="O14" s="69"/>
+      <c r="N14" s="76"/>
+      <c r="O14" s="77"/>
       <c r="P14" s="55"/>
       <c r="S14" s="12"/>
       <c r="T14" s="12"/>
@@ -2713,8 +2713,8 @@
       <c r="Y14" s="11"/>
       <c r="Z14" s="11"/>
       <c r="AA14" s="11"/>
-      <c r="AB14" s="68"/>
-      <c r="AC14" s="69"/>
+      <c r="AB14" s="76"/>
+      <c r="AC14" s="77"/>
       <c r="AD14" s="11"/>
       <c r="AE14" s="55"/>
     </row>
@@ -2722,7 +2722,7 @@
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="82"/>
+      <c r="C15" s="92"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="G15" s="12">
@@ -2734,8 +2734,8 @@
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
-      <c r="N15" s="64"/>
-      <c r="O15" s="65"/>
+      <c r="N15" s="74"/>
+      <c r="O15" s="75"/>
       <c r="P15" s="55"/>
       <c r="S15" s="12"/>
       <c r="T15" s="12"/>
@@ -2746,8 +2746,8 @@
       <c r="Y15" s="11"/>
       <c r="Z15" s="11"/>
       <c r="AA15" s="11"/>
-      <c r="AB15" s="64"/>
-      <c r="AC15" s="65"/>
+      <c r="AB15" s="74"/>
+      <c r="AC15" s="75"/>
       <c r="AD15" s="11"/>
       <c r="AE15" s="55"/>
     </row>
@@ -2755,7 +2755,7 @@
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="82"/>
+      <c r="C16" s="92"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="G16" s="12"/>
@@ -2765,8 +2765,8 @@
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
-      <c r="N16" s="64"/>
-      <c r="O16" s="65"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="75"/>
       <c r="P16" s="55"/>
       <c r="S16" s="12"/>
       <c r="T16" s="12"/>
@@ -2777,8 +2777,8 @@
       <c r="Y16" s="11"/>
       <c r="Z16" s="11"/>
       <c r="AA16" s="11"/>
-      <c r="AB16" s="64"/>
-      <c r="AC16" s="65"/>
+      <c r="AB16" s="74"/>
+      <c r="AC16" s="75"/>
       <c r="AD16" s="11"/>
       <c r="AE16" s="55"/>
     </row>
@@ -2786,7 +2786,7 @@
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="82"/>
+      <c r="C17" s="92"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="G17" s="12"/>
@@ -2796,8 +2796,8 @@
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
-      <c r="N17" s="64"/>
-      <c r="O17" s="65"/>
+      <c r="N17" s="74"/>
+      <c r="O17" s="75"/>
       <c r="P17" s="55"/>
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
@@ -2808,8 +2808,8 @@
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
       <c r="AA17" s="11"/>
-      <c r="AB17" s="64"/>
-      <c r="AC17" s="65"/>
+      <c r="AB17" s="74"/>
+      <c r="AC17" s="75"/>
       <c r="AD17" s="11"/>
       <c r="AE17" s="55"/>
     </row>
@@ -2817,7 +2817,7 @@
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="82"/>
+      <c r="C18" s="92"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="G18" s="12"/>
@@ -2827,8 +2827,8 @@
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
-      <c r="N18" s="64"/>
-      <c r="O18" s="65"/>
+      <c r="N18" s="74"/>
+      <c r="O18" s="75"/>
       <c r="P18" s="55"/>
       <c r="S18" s="12"/>
       <c r="T18" s="12"/>
@@ -2839,8 +2839,8 @@
       <c r="Y18" s="11"/>
       <c r="Z18" s="11"/>
       <c r="AA18" s="11"/>
-      <c r="AB18" s="64"/>
-      <c r="AC18" s="65"/>
+      <c r="AB18" s="74"/>
+      <c r="AC18" s="75"/>
       <c r="AD18" s="11"/>
       <c r="AE18" s="55"/>
     </row>
@@ -2848,7 +2848,7 @@
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="82"/>
+      <c r="C19" s="92"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="G19" s="13"/>
@@ -2858,8 +2858,8 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="64"/>
-      <c r="O19" s="65"/>
+      <c r="N19" s="74"/>
+      <c r="O19" s="75"/>
       <c r="P19" s="55"/>
       <c r="S19" s="13"/>
       <c r="T19" s="13"/>
@@ -2870,8 +2870,8 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
-      <c r="AB19" s="64"/>
-      <c r="AC19" s="65"/>
+      <c r="AB19" s="74"/>
+      <c r="AC19" s="75"/>
       <c r="AD19" s="11"/>
       <c r="AE19" s="55"/>
     </row>
@@ -2879,7 +2879,7 @@
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="82"/>
+      <c r="C20" s="92"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
@@ -2887,29 +2887,30 @@
       <c r="D22" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="88"/>
-      <c r="G22" s="88"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="G5:P5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="AB9:AC9"/>
+    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="AB11:AC11"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="S5:AE5"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="AB7:AC7"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C19:C20"/>
@@ -2918,25 +2919,24 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="S5:AE5"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="AB8:AC8"/>
-    <mergeCell ref="AB9:AC9"/>
-    <mergeCell ref="AB10:AC10"/>
-    <mergeCell ref="AB11:AC11"/>
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="G5:P5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N18:O18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2973,12 +2973,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="58" t="s">
@@ -2991,25 +2991,25 @@
       <c r="G3" s="50"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="96"/>
+      <c r="M5" s="96"/>
+      <c r="N5" s="96"/>
+      <c r="O5" s="96"/>
+      <c r="P5" s="97"/>
     </row>
     <row r="6" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -3047,10 +3047,10 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="83">
+      <c r="B7" s="90">
         <v>1</v>
       </c>
-      <c r="C7" s="89" t="s">
+      <c r="C7" s="100" t="s">
         <v>90</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -3083,18 +3083,18 @@
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="87"/>
-      <c r="C8" s="90"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="101"/>
       <c r="D8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="132">
+      <c r="F8" s="65">
         <v>1</v>
       </c>
-      <c r="G8" s="132">
+      <c r="G8" s="65">
         <v>3</v>
       </c>
-      <c r="H8" s="132" t="s">
+      <c r="H8" s="65" t="s">
         <v>76</v>
       </c>
       <c r="I8" s="21" t="s">
@@ -3115,7 +3115,7 @@
       <c r="N8" s="21">
         <v>10</v>
       </c>
-      <c r="O8" s="135" t="s">
+      <c r="O8" s="67" t="s">
         <v>89</v>
       </c>
       <c r="P8" s="56" t="s">
@@ -3123,18 +3123,18 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="87"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="131" t="s">
+      <c r="B9" s="91"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="132">
+      <c r="F9" s="65">
         <v>2</v>
       </c>
-      <c r="G9" s="132">
+      <c r="G9" s="65">
         <v>1</v>
       </c>
-      <c r="H9" s="132" t="s">
+      <c r="H9" s="65" t="s">
         <v>100</v>
       </c>
       <c r="I9" s="21" t="s">
@@ -3155,7 +3155,7 @@
       <c r="N9" s="21">
         <v>10</v>
       </c>
-      <c r="O9" s="135" t="s">
+      <c r="O9" s="67" t="s">
         <v>89</v>
       </c>
       <c r="P9" s="56" t="s">
@@ -3163,18 +3163,18 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="87"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="131" t="s">
+      <c r="B10" s="91"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="132">
+      <c r="F10" s="65">
         <v>3</v>
       </c>
-      <c r="G10" s="132">
+      <c r="G10" s="65">
         <v>8</v>
       </c>
-      <c r="H10" s="132" t="s">
+      <c r="H10" s="65" t="s">
         <v>101</v>
       </c>
       <c r="I10" s="21" t="s">
@@ -3195,7 +3195,7 @@
       <c r="N10" s="21">
         <v>10</v>
       </c>
-      <c r="O10" s="135" t="s">
+      <c r="O10" s="67" t="s">
         <v>89</v>
       </c>
       <c r="P10" s="56" t="s">
@@ -3203,18 +3203,18 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="87"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="131" t="s">
+      <c r="B11" s="91"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="132">
+      <c r="F11" s="65">
         <v>4</v>
       </c>
-      <c r="G11" s="132">
+      <c r="G11" s="65">
         <v>7</v>
       </c>
-      <c r="H11" s="132" t="s">
+      <c r="H11" s="65" t="s">
         <v>77</v>
       </c>
       <c r="I11" s="21" t="s">
@@ -3235,7 +3235,7 @@
       <c r="N11" s="21">
         <v>10</v>
       </c>
-      <c r="O11" s="135" t="s">
+      <c r="O11" s="67" t="s">
         <v>89</v>
       </c>
       <c r="P11" s="56" t="s">
@@ -3243,124 +3243,124 @@
       </c>
     </row>
     <row r="12" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="84"/>
-      <c r="C12" s="91"/>
+      <c r="B12" s="93"/>
+      <c r="C12" s="102"/>
       <c r="D12" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F12" s="132">
+      <c r="F12" s="65">
         <v>5</v>
       </c>
-      <c r="G12" s="132"/>
-      <c r="H12" s="132"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
       <c r="I12" s="21"/>
       <c r="J12" s="21"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="135"/>
+      <c r="O12" s="67"/>
       <c r="P12" s="56"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="83">
+      <c r="B13" s="90">
         <v>2</v>
       </c>
-      <c r="C13" s="83" t="s">
+      <c r="C13" s="90" t="s">
         <v>83</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F13" s="132">
+      <c r="F13" s="65">
         <v>6</v>
       </c>
-      <c r="G13" s="132"/>
-      <c r="H13" s="132"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
       <c r="I13" s="21"/>
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
-      <c r="O13" s="133"/>
+      <c r="O13" s="63"/>
       <c r="P13" s="56"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="87"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="131" t="s">
+      <c r="B14" s="91"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="132">
+      <c r="F14" s="65">
         <v>7</v>
       </c>
-      <c r="G14" s="132"/>
-      <c r="H14" s="132"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="134"/>
+      <c r="O14" s="66"/>
       <c r="P14" s="56"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="87"/>
-      <c r="C15" s="87"/>
-      <c r="D15" s="131" t="s">
+      <c r="B15" s="91"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="F15" s="132">
+      <c r="F15" s="65">
         <v>8</v>
       </c>
-      <c r="G15" s="132"/>
-      <c r="H15" s="132"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
       <c r="I15" s="21"/>
       <c r="J15" s="21"/>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
-      <c r="O15" s="133"/>
+      <c r="O15" s="63"/>
       <c r="P15" s="56"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="87"/>
-      <c r="C16" s="87"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="91"/>
       <c r="D16" s="2"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="132"/>
-      <c r="H16" s="132"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
       <c r="I16" s="21"/>
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="133"/>
+      <c r="O16" s="63"/>
       <c r="P16" s="56"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="87"/>
-      <c r="C17" s="87"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="91"/>
       <c r="D17" s="2"/>
-      <c r="F17" s="132"/>
-      <c r="G17" s="132"/>
-      <c r="H17" s="132"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
       <c r="I17" s="21"/>
       <c r="J17" s="21"/>
       <c r="K17" s="21"/>
       <c r="L17" s="21"/>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
-      <c r="O17" s="133"/>
+      <c r="O17" s="63"/>
       <c r="P17" s="56"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="84"/>
-      <c r="C18" s="84"/>
+      <c r="B18" s="93"/>
+      <c r="C18" s="93"/>
       <c r="D18" s="2"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
@@ -3375,10 +3375,10 @@
       <c r="P18" s="55"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="83">
+      <c r="B19" s="90">
         <v>3</v>
       </c>
-      <c r="C19" s="89"/>
+      <c r="C19" s="100"/>
       <c r="D19" s="2"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
@@ -3393,66 +3393,67 @@
       <c r="P19" s="55"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="87"/>
-      <c r="C20" s="90"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="101"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="87"/>
-      <c r="C21" s="90"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="101"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="87"/>
-      <c r="C22" s="90"/>
+      <c r="B22" s="91"/>
+      <c r="C22" s="101"/>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="87"/>
-      <c r="C23" s="90"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="101"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="84"/>
-      <c r="C24" s="91"/>
+      <c r="B24" s="93"/>
+      <c r="C24" s="102"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="83">
+      <c r="B25" s="90">
         <v>4</v>
       </c>
-      <c r="C25" s="89"/>
+      <c r="C25" s="100"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="87"/>
-      <c r="C26" s="90"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="101"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="87"/>
-      <c r="C27" s="90"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="101"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="87"/>
-      <c r="C28" s="90"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="101"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="87"/>
-      <c r="C29" s="90"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="101"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="84"/>
-      <c r="C30" s="91"/>
+      <c r="B30" s="93"/>
+      <c r="C30" s="102"/>
       <c r="D30" s="2" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="F5:P5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B25:B30"/>
     <mergeCell ref="C25:C30"/>
@@ -3463,7 +3464,6 @@
     <mergeCell ref="C19:C24"/>
     <mergeCell ref="B19:B24"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F5:P5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3479,7 +3479,7 @@
   <dimension ref="B1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3496,64 +3496,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="132" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100"/>
-      <c r="O3" s="100"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="132"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="132"/>
+      <c r="M3" s="132"/>
+      <c r="N3" s="132"/>
+      <c r="O3" s="132"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="106" t="s">
+      <c r="D4" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="96" t="s">
+      <c r="E4" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="133" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="79" t="s">
+      <c r="G4" s="134"/>
+      <c r="H4" s="134"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="134"/>
+      <c r="L4" s="134"/>
+      <c r="M4" s="135"/>
+      <c r="N4" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="O4" s="81"/>
+      <c r="O4" s="83"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="105"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="97"/>
+      <c r="B5" s="116"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="129"/>
       <c r="F5" s="13" t="s">
         <v>62</v>
       </c>
@@ -3569,11 +3569,11 @@
       <c r="J5" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="K5" s="79" t="s">
+      <c r="K5" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="80"/>
-      <c r="M5" s="81"/>
+      <c r="L5" s="87"/>
+      <c r="M5" s="83"/>
       <c r="N5" s="51" t="s">
         <v>31</v>
       </c>
@@ -3585,7 +3585,7 @@
       <c r="B6" s="14">
         <v>1</v>
       </c>
-      <c r="C6" s="102" t="s">
+      <c r="C6" s="113" t="s">
         <v>48</v>
       </c>
       <c r="D6" s="18"/>
@@ -3599,7 +3599,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I6" s="21">
         <v>0</v>
@@ -3607,16 +3607,16 @@
       <c r="J6" s="21">
         <v>10</v>
       </c>
-      <c r="K6" s="129" t="s">
+      <c r="K6" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="L6" s="136"/>
-      <c r="M6" s="130"/>
+      <c r="L6" s="104"/>
+      <c r="M6" s="81"/>
       <c r="N6" s="56" t="s">
         <v>74</v>
       </c>
       <c r="O6" s="56" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -3624,7 +3624,7 @@
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="102"/>
+      <c r="C7" s="113"/>
       <c r="D7" s="19"/>
       <c r="E7" s="8">
         <v>3</v>
@@ -3636,7 +3636,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I7" s="21">
         <v>0</v>
@@ -3644,11 +3644,11 @@
       <c r="J7" s="21">
         <v>10</v>
       </c>
-      <c r="K7" s="129" t="s">
+      <c r="K7" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="L7" s="136"/>
-      <c r="M7" s="130"/>
+      <c r="L7" s="104"/>
+      <c r="M7" s="81"/>
       <c r="N7" s="56" t="s">
         <v>103</v>
       </c>
@@ -3661,7 +3661,7 @@
         <f t="shared" ref="B8:B13" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="102"/>
+      <c r="C8" s="113"/>
       <c r="D8" s="19"/>
       <c r="E8" s="8">
         <v>8</v>
@@ -3681,11 +3681,11 @@
       <c r="J8" s="21">
         <v>10</v>
       </c>
-      <c r="K8" s="129" t="s">
+      <c r="K8" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="L8" s="136"/>
-      <c r="M8" s="130"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="81"/>
       <c r="N8" s="56" t="s">
         <v>103</v>
       </c>
@@ -3698,7 +3698,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="102"/>
+      <c r="C9" s="113"/>
       <c r="D9" s="19"/>
       <c r="E9" s="8">
         <v>9</v>
@@ -3718,11 +3718,11 @@
       <c r="J9" s="21">
         <v>10</v>
       </c>
-      <c r="K9" s="129" t="s">
+      <c r="K9" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="L9" s="136"/>
-      <c r="M9" s="130"/>
+      <c r="L9" s="104"/>
+      <c r="M9" s="81"/>
       <c r="N9" s="56" t="s">
         <v>103</v>
       </c>
@@ -3735,7 +3735,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="102"/>
+      <c r="C10" s="113"/>
       <c r="D10" s="19">
         <v>1</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I10" s="21">
         <v>0</v>
@@ -3755,11 +3755,11 @@
       <c r="J10" s="21">
         <v>10</v>
       </c>
-      <c r="K10" s="129" t="s">
+      <c r="K10" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="L10" s="136"/>
-      <c r="M10" s="130"/>
+      <c r="L10" s="104"/>
+      <c r="M10" s="81"/>
       <c r="N10" s="56" t="s">
         <v>103</v>
       </c>
@@ -3772,7 +3772,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="102"/>
+      <c r="C11" s="113"/>
       <c r="D11" s="19">
         <v>2</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I11" s="21">
         <v>0</v>
@@ -3792,16 +3792,16 @@
       <c r="J11" s="21">
         <v>10</v>
       </c>
-      <c r="K11" s="129" t="s">
+      <c r="K11" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="L11" s="136"/>
-      <c r="M11" s="130"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="81"/>
       <c r="N11" s="56" t="s">
         <v>74</v>
       </c>
       <c r="O11" s="56" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
@@ -3809,7 +3809,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="102"/>
+      <c r="C12" s="113"/>
       <c r="D12" s="19">
         <v>3</v>
       </c>
@@ -3829,16 +3829,16 @@
       <c r="J12" s="21">
         <v>10</v>
       </c>
-      <c r="K12" s="129" t="s">
+      <c r="K12" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="L12" s="136"/>
-      <c r="M12" s="130"/>
+      <c r="L12" s="104"/>
+      <c r="M12" s="81"/>
       <c r="N12" s="56" t="s">
         <v>74</v>
       </c>
       <c r="O12" s="56" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3846,7 +3846,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="103"/>
+      <c r="C13" s="114"/>
       <c r="D13" s="20">
         <v>4</v>
       </c>
@@ -3866,11 +3866,11 @@
       <c r="J13" s="21">
         <v>10</v>
       </c>
-      <c r="K13" s="129" t="s">
+      <c r="K13" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="L13" s="136"/>
-      <c r="M13" s="130"/>
+      <c r="L13" s="104"/>
+      <c r="M13" s="81"/>
       <c r="N13" s="56" t="s">
         <v>103</v>
       </c>
@@ -3905,98 +3905,98 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="101"/>
-      <c r="L15" s="101"/>
+      <c r="K15" s="136"/>
+      <c r="L15" s="136"/>
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="114" t="s">
+      <c r="C17" s="107" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="115"/>
-      <c r="E17" s="115"/>
-      <c r="F17" s="116"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="110"/>
       <c r="G17" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="H17" s="114" t="s">
+      <c r="H17" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="117"/>
-      <c r="J17" s="115"/>
-      <c r="K17" s="115"/>
-      <c r="L17" s="116"/>
-      <c r="M17" s="114" t="s">
+      <c r="I17" s="108"/>
+      <c r="J17" s="109"/>
+      <c r="K17" s="109"/>
+      <c r="L17" s="110"/>
+      <c r="M17" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="N17" s="117"/>
-      <c r="O17" s="115"/>
-      <c r="P17" s="116"/>
+      <c r="N17" s="108"/>
+      <c r="O17" s="109"/>
+      <c r="P17" s="110"/>
     </row>
     <row r="18" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="110" t="s">
+      <c r="B18" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="111" t="s">
+      <c r="C18" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="112" t="s">
+      <c r="D18" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="112" t="s">
+      <c r="E18" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="113" t="s">
+      <c r="F18" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="122" t="s">
+      <c r="G18" s="127" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="118" t="s">
+      <c r="H18" s="123" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="119"/>
-      <c r="J18" s="112" t="s">
+      <c r="I18" s="124"/>
+      <c r="J18" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="K18" s="112" t="s">
+      <c r="K18" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="L18" s="113" t="s">
+      <c r="L18" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="M18" s="123" t="s">
+      <c r="M18" s="111" t="s">
         <v>59</v>
       </c>
-      <c r="N18" s="112" t="s">
+      <c r="N18" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="O18" s="112" t="s">
+      <c r="O18" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="P18" s="113" t="s">
+      <c r="P18" s="106" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="110"/>
-      <c r="C19" s="111"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="112"/>
-      <c r="F19" s="113"/>
-      <c r="G19" s="122"/>
-      <c r="H19" s="120"/>
-      <c r="I19" s="121"/>
-      <c r="J19" s="112"/>
-      <c r="K19" s="112"/>
-      <c r="L19" s="113"/>
-      <c r="M19" s="124"/>
-      <c r="N19" s="112"/>
-      <c r="O19" s="112"/>
-      <c r="P19" s="113"/>
+      <c r="B19" s="121"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="105"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="127"/>
+      <c r="H19" s="125"/>
+      <c r="I19" s="126"/>
+      <c r="J19" s="105"/>
+      <c r="K19" s="105"/>
+      <c r="L19" s="106"/>
+      <c r="M19" s="112"/>
+      <c r="N19" s="105"/>
+      <c r="O19" s="105"/>
+      <c r="P19" s="106"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="28" t="s">
@@ -4017,10 +4017,10 @@
       <c r="G20" s="30">
         <v>4</v>
       </c>
-      <c r="H20" s="108" t="s">
+      <c r="H20" s="119" t="s">
         <v>73</v>
       </c>
-      <c r="I20" s="109"/>
+      <c r="I20" s="120"/>
       <c r="J20" s="2">
         <v>4</v>
       </c>
@@ -4052,8 +4052,8 @@
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
-      <c r="L33" s="64"/>
-      <c r="M33" s="65"/>
+      <c r="L33" s="74"/>
+      <c r="M33" s="75"/>
       <c r="N33" s="11"/>
       <c r="O33" s="55"/>
     </row>
@@ -4063,8 +4063,8 @@
       <c r="I34" s="11"/>
       <c r="J34" s="11"/>
       <c r="K34" s="11"/>
-      <c r="L34" s="64"/>
-      <c r="M34" s="65"/>
+      <c r="L34" s="74"/>
+      <c r="M34" s="75"/>
       <c r="N34" s="11"/>
       <c r="O34" s="55"/>
     </row>
@@ -4074,8 +4074,8 @@
       <c r="I35" s="11"/>
       <c r="J35" s="11"/>
       <c r="K35" s="11"/>
-      <c r="L35" s="64"/>
-      <c r="M35" s="65"/>
+      <c r="L35" s="74"/>
+      <c r="M35" s="75"/>
       <c r="N35" s="11"/>
       <c r="O35" s="55"/>
     </row>
@@ -4085,26 +4085,26 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" s="64"/>
-      <c r="M36" s="65"/>
+      <c r="L36" s="74"/>
+      <c r="M36" s="75"/>
       <c r="N36" s="11"/>
       <c r="O36" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="F4:M4"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="C6:C13"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
@@ -4120,19 +4120,19 @@
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="K18:K19"/>
     <mergeCell ref="L18:L19"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="F4:M4"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
   </mergeCells>
   <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4142,18 +4142,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4301,6 +4301,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="c46c0853-0d59-45c6-b517-3e25eac8cdf1"/>
@@ -4312,14 +4320,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updated excel to reflect test
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form_Pedestro.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form_Pedestro.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD39F3F-ADD2-46F6-9E21-59AF0187EDBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF63A0A-4544-41AF-B9A5-7136506E8935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="690" windowWidth="28800" windowHeight="15885" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="M15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="105">
   <si>
     <t>VVSS, Info Romana, 2023-2024</t>
   </si>
@@ -676,6 +676,9 @@
   </si>
   <si>
     <t>success</t>
+  </si>
+  <si>
+    <t>1,3</t>
   </si>
 </sst>
 </file>
@@ -873,7 +876,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -940,8 +943,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="33">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -978,16 +987,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -997,34 +1002,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1359,7 +1340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1391,22 +1372,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1414,19 +1389,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1435,23 +1410,23 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1472,247 +1447,245 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2036,24 +2009,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="71"/>
-      <c r="H1" s="35" t="s">
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="69"/>
+      <c r="H1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H2" s="72" t="s">
+      <c r="H2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H3" s="2"/>
@@ -2079,7 +2052,7 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
+      <c r="B6" s="21"/>
       <c r="H6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2088,7 +2061,7 @@
     </row>
     <row r="7" spans="2:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="31" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2149,7 +2122,7 @@
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="31" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2159,7 +2132,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="29" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2203,25 +2176,25 @@
       <c r="O23" s="1"/>
     </row>
     <row r="24" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="68" t="s">
+      <c r="A24" s="30"/>
+      <c r="B24" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="68"/>
-      <c r="N24" s="68"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
+      <c r="J24" s="66"/>
+      <c r="K24" s="66"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="66"/>
+      <c r="N24" s="66"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C26" s="34"/>
+      <c r="C26" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2263,55 +2236,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="71"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="3" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="50"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48"/>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="93" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="G5" s="84" t="s">
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="G5" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="84"/>
-      <c r="S5" s="95"/>
-      <c r="T5" s="96"/>
-      <c r="U5" s="96"/>
-      <c r="V5" s="96"/>
-      <c r="W5" s="96"/>
-      <c r="X5" s="96"/>
-      <c r="Y5" s="96"/>
-      <c r="Z5" s="96"/>
-      <c r="AA5" s="96"/>
-      <c r="AB5" s="96"/>
-      <c r="AC5" s="96"/>
-      <c r="AD5" s="96"/>
-      <c r="AE5" s="97"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="94"/>
+      <c r="N5" s="94"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="80"/>
+      <c r="U5" s="80"/>
+      <c r="V5" s="80"/>
+      <c r="W5" s="80"/>
+      <c r="X5" s="80"/>
+      <c r="Y5" s="80"/>
+      <c r="Z5" s="80"/>
+      <c r="AA5" s="80"/>
+      <c r="AB5" s="80"/>
+      <c r="AC5" s="80"/>
+      <c r="AD5" s="80"/>
+      <c r="AE5" s="81"/>
     </row>
     <row r="6" spans="2:31" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
@@ -2326,13 +2299,13 @@
       <c r="E6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="85" t="s">
+      <c r="G6" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="88" t="s">
+      <c r="H6" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="82" t="s">
+      <c r="I6" s="86" t="s">
         <v>30</v>
       </c>
       <c r="J6" s="87"/>
@@ -2341,36 +2314,36 @@
       <c r="M6" s="87"/>
       <c r="N6" s="87"/>
       <c r="O6" s="87"/>
-      <c r="P6" s="51" t="s">
+      <c r="P6" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="S6" s="85"/>
-      <c r="T6" s="85"/>
-      <c r="U6" s="85"/>
-      <c r="V6" s="88"/>
-      <c r="W6" s="82"/>
+      <c r="S6" s="82"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="82"/>
+      <c r="V6" s="84"/>
+      <c r="W6" s="86"/>
       <c r="X6" s="87"/>
       <c r="Y6" s="87"/>
       <c r="Z6" s="87"/>
       <c r="AA6" s="87"/>
       <c r="AB6" s="87"/>
       <c r="AC6" s="87"/>
-      <c r="AD6" s="83"/>
-      <c r="AE6" s="51"/>
+      <c r="AD6" s="88"/>
+      <c r="AE6" s="49"/>
     </row>
     <row r="7" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="92" t="s">
+      <c r="C7" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="45" t="s">
         <v>60</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="89"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="85"/>
       <c r="I7" s="13" t="s">
         <v>62</v>
       </c>
@@ -2386,64 +2359,64 @@
       <c r="M7" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="N7" s="82" t="s">
+      <c r="N7" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="O7" s="83"/>
-      <c r="P7" s="51" t="s">
+      <c r="O7" s="88"/>
+      <c r="P7" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="S7" s="86"/>
-      <c r="T7" s="86"/>
-      <c r="U7" s="86"/>
-      <c r="V7" s="89"/>
+      <c r="S7" s="83"/>
+      <c r="T7" s="83"/>
+      <c r="U7" s="83"/>
+      <c r="V7" s="85"/>
       <c r="W7" s="13"/>
       <c r="X7" s="13"/>
       <c r="Y7" s="13"/>
       <c r="Z7" s="13"/>
       <c r="AA7" s="13"/>
-      <c r="AB7" s="82"/>
-      <c r="AC7" s="83"/>
-      <c r="AD7" s="52"/>
-      <c r="AE7" s="51"/>
+      <c r="AB7" s="86"/>
+      <c r="AC7" s="88"/>
+      <c r="AD7" s="50"/>
+      <c r="AE7" s="49"/>
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="92"/>
+      <c r="C8" s="91"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="44" t="s">
         <v>82</v>
       </c>
       <c r="G8" s="13">
         <v>1</v>
       </c>
-      <c r="H8" s="60" t="s">
+      <c r="H8" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="19">
         <v>1</v>
       </c>
-      <c r="K8" s="21">
+      <c r="K8" s="19">
         <v>1</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="19">
         <v>1</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="19">
         <v>10</v>
       </c>
-      <c r="N8" s="80" t="s">
+      <c r="N8" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="O8" s="81" t="s">
+      <c r="O8" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="56" t="s">
+      <c r="P8" s="54" t="s">
         <v>70</v>
       </c>
       <c r="S8" s="13"/>
@@ -2455,50 +2428,50 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
-      <c r="AB8" s="74"/>
-      <c r="AC8" s="75"/>
+      <c r="AB8" s="71"/>
+      <c r="AC8" s="72"/>
       <c r="AD8" s="2"/>
-      <c r="AE8" s="50"/>
+      <c r="AE8" s="48"/>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="90" t="s">
+      <c r="C9" s="89" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="47" t="s">
+      <c r="D9" s="45" t="s">
         <v>84</v>
       </c>
       <c r="E9" s="4"/>
       <c r="G9" s="13">
         <v>2</v>
       </c>
-      <c r="H9" s="61" t="s">
+      <c r="H9" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="19">
         <v>1</v>
       </c>
-      <c r="K9" s="21">
+      <c r="K9" s="19">
         <v>1</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="19">
         <v>1</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="19">
         <v>10</v>
       </c>
-      <c r="N9" s="80" t="s">
+      <c r="N9" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="O9" s="81" t="s">
+      <c r="O9" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="P9" s="56" t="s">
+      <c r="P9" s="54" t="s">
         <v>72</v>
       </c>
       <c r="S9" s="13"/>
@@ -2510,120 +2483,120 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
-      <c r="AB9" s="74"/>
-      <c r="AC9" s="75"/>
+      <c r="AB9" s="71"/>
+      <c r="AC9" s="72"/>
       <c r="AD9" s="2"/>
-      <c r="AE9" s="50"/>
+      <c r="AE9" s="48"/>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="91"/>
+      <c r="C10" s="90"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="20">
         <v>3</v>
       </c>
-      <c r="H10" s="62" t="s">
+      <c r="H10" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="19">
         <v>1</v>
       </c>
-      <c r="K10" s="21">
+      <c r="K10" s="19">
         <v>-1</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="19">
         <v>1</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="19">
         <v>10</v>
       </c>
-      <c r="N10" s="80" t="s">
+      <c r="N10" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="O10" s="81" t="s">
+      <c r="O10" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="P10" s="56" t="s">
+      <c r="P10" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="22"/>
-      <c r="V10" s="21"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="19"/>
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
       <c r="AA10" s="10"/>
-      <c r="AB10" s="98"/>
-      <c r="AC10" s="99"/>
+      <c r="AB10" s="77"/>
+      <c r="AC10" s="78"/>
       <c r="AD10" s="10"/>
-      <c r="AE10" s="56"/>
+      <c r="AE10" s="54"/>
     </row>
     <row r="11" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="43"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="59"/>
-      <c r="G11" s="22">
+      <c r="E11" s="57"/>
+      <c r="G11" s="20">
         <v>4</v>
       </c>
-      <c r="H11" s="62" t="s">
+      <c r="H11" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="19">
         <v>1</v>
       </c>
-      <c r="K11" s="21">
+      <c r="K11" s="19">
         <v>-1</v>
       </c>
-      <c r="L11" s="21">
+      <c r="L11" s="19">
         <v>1</v>
       </c>
-      <c r="M11" s="21">
+      <c r="M11" s="19">
         <v>10</v>
       </c>
-      <c r="N11" s="80" t="s">
+      <c r="N11" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="O11" s="81" t="s">
+      <c r="O11" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="P11" s="56" t="s">
+      <c r="P11" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
-      <c r="U11" s="22"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
       <c r="AA11" s="10"/>
-      <c r="AB11" s="98"/>
-      <c r="AC11" s="99"/>
+      <c r="AB11" s="77"/>
+      <c r="AC11" s="78"/>
       <c r="AD11" s="10"/>
-      <c r="AE11" s="53"/>
+      <c r="AE11" s="51"/>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="44"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="G12" s="9">
@@ -2635,9 +2608,9 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="78"/>
-      <c r="O12" s="79"/>
-      <c r="P12" s="54"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="74"/>
+      <c r="P12" s="52"/>
       <c r="S12" s="9"/>
       <c r="T12" s="9"/>
       <c r="U12" s="9"/>
@@ -2647,16 +2620,16 @@
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
-      <c r="AB12" s="78"/>
-      <c r="AC12" s="79"/>
+      <c r="AB12" s="73"/>
+      <c r="AC12" s="74"/>
       <c r="AD12" s="6"/>
-      <c r="AE12" s="54"/>
+      <c r="AE12" s="52"/>
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="90"/>
+      <c r="C13" s="89"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="G13" s="9">
@@ -2668,9 +2641,9 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
-      <c r="N13" s="78"/>
-      <c r="O13" s="79"/>
-      <c r="P13" s="54"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="74"/>
+      <c r="P13" s="52"/>
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
       <c r="U13" s="9"/>
@@ -2680,16 +2653,16 @@
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
       <c r="AA13" s="6"/>
-      <c r="AB13" s="78"/>
-      <c r="AC13" s="79"/>
+      <c r="AB13" s="73"/>
+      <c r="AC13" s="74"/>
       <c r="AD13" s="6"/>
-      <c r="AE13" s="54"/>
+      <c r="AE13" s="52"/>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="93"/>
+      <c r="C14" s="92"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="G14" s="12">
@@ -2701,9 +2674,9 @@
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
-      <c r="N14" s="76"/>
-      <c r="O14" s="77"/>
-      <c r="P14" s="55"/>
+      <c r="N14" s="75"/>
+      <c r="O14" s="76"/>
+      <c r="P14" s="53"/>
       <c r="S14" s="12"/>
       <c r="T14" s="12"/>
       <c r="U14" s="12"/>
@@ -2713,16 +2686,16 @@
       <c r="Y14" s="11"/>
       <c r="Z14" s="11"/>
       <c r="AA14" s="11"/>
-      <c r="AB14" s="76"/>
-      <c r="AC14" s="77"/>
+      <c r="AB14" s="75"/>
+      <c r="AC14" s="76"/>
       <c r="AD14" s="11"/>
-      <c r="AE14" s="55"/>
+      <c r="AE14" s="53"/>
     </row>
     <row r="15" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="92"/>
+      <c r="C15" s="91"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="G15" s="12">
@@ -2734,9 +2707,9 @@
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
-      <c r="N15" s="74"/>
-      <c r="O15" s="75"/>
-      <c r="P15" s="55"/>
+      <c r="N15" s="71"/>
+      <c r="O15" s="72"/>
+      <c r="P15" s="53"/>
       <c r="S15" s="12"/>
       <c r="T15" s="12"/>
       <c r="U15" s="12"/>
@@ -2746,16 +2719,16 @@
       <c r="Y15" s="11"/>
       <c r="Z15" s="11"/>
       <c r="AA15" s="11"/>
-      <c r="AB15" s="74"/>
-      <c r="AC15" s="75"/>
+      <c r="AB15" s="71"/>
+      <c r="AC15" s="72"/>
       <c r="AD15" s="11"/>
-      <c r="AE15" s="55"/>
+      <c r="AE15" s="53"/>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="92"/>
+      <c r="C16" s="91"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="G16" s="12"/>
@@ -2765,9 +2738,9 @@
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
-      <c r="N16" s="74"/>
-      <c r="O16" s="75"/>
-      <c r="P16" s="55"/>
+      <c r="N16" s="71"/>
+      <c r="O16" s="72"/>
+      <c r="P16" s="53"/>
       <c r="S16" s="12"/>
       <c r="T16" s="12"/>
       <c r="U16" s="12"/>
@@ -2777,16 +2750,16 @@
       <c r="Y16" s="11"/>
       <c r="Z16" s="11"/>
       <c r="AA16" s="11"/>
-      <c r="AB16" s="74"/>
-      <c r="AC16" s="75"/>
+      <c r="AB16" s="71"/>
+      <c r="AC16" s="72"/>
       <c r="AD16" s="11"/>
-      <c r="AE16" s="55"/>
+      <c r="AE16" s="53"/>
     </row>
     <row r="17" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="92"/>
+      <c r="C17" s="91"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="G17" s="12"/>
@@ -2796,9 +2769,9 @@
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
-      <c r="N17" s="74"/>
-      <c r="O17" s="75"/>
-      <c r="P17" s="55"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="72"/>
+      <c r="P17" s="53"/>
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
       <c r="U17" s="12"/>
@@ -2808,16 +2781,16 @@
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
       <c r="AA17" s="11"/>
-      <c r="AB17" s="74"/>
-      <c r="AC17" s="75"/>
+      <c r="AB17" s="71"/>
+      <c r="AC17" s="72"/>
       <c r="AD17" s="11"/>
-      <c r="AE17" s="55"/>
+      <c r="AE17" s="53"/>
     </row>
     <row r="18" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="92"/>
+      <c r="C18" s="91"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="G18" s="12"/>
@@ -2827,9 +2800,9 @@
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
-      <c r="N18" s="74"/>
-      <c r="O18" s="75"/>
-      <c r="P18" s="55"/>
+      <c r="N18" s="71"/>
+      <c r="O18" s="72"/>
+      <c r="P18" s="53"/>
       <c r="S18" s="12"/>
       <c r="T18" s="12"/>
       <c r="U18" s="12"/>
@@ -2839,16 +2812,16 @@
       <c r="Y18" s="11"/>
       <c r="Z18" s="11"/>
       <c r="AA18" s="11"/>
-      <c r="AB18" s="74"/>
-      <c r="AC18" s="75"/>
+      <c r="AB18" s="71"/>
+      <c r="AC18" s="72"/>
       <c r="AD18" s="11"/>
-      <c r="AE18" s="55"/>
+      <c r="AE18" s="53"/>
     </row>
     <row r="19" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="92"/>
+      <c r="C19" s="91"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="G19" s="13"/>
@@ -2858,9 +2831,9 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="74"/>
-      <c r="O19" s="75"/>
-      <c r="P19" s="55"/>
+      <c r="N19" s="71"/>
+      <c r="O19" s="72"/>
+      <c r="P19" s="53"/>
       <c r="S19" s="13"/>
       <c r="T19" s="13"/>
       <c r="U19" s="13"/>
@@ -2870,16 +2843,16 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
-      <c r="AB19" s="74"/>
-      <c r="AC19" s="75"/>
+      <c r="AB19" s="71"/>
+      <c r="AC19" s="72"/>
       <c r="AD19" s="11"/>
-      <c r="AE19" s="55"/>
+      <c r="AE19" s="53"/>
     </row>
     <row r="20" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="92"/>
+      <c r="C20" s="91"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
@@ -2887,30 +2860,29 @@
       <c r="D22" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
+      <c r="F22" s="97"/>
+      <c r="G22" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB8:AC8"/>
-    <mergeCell ref="AB9:AC9"/>
-    <mergeCell ref="AB10:AC10"/>
-    <mergeCell ref="AB11:AC11"/>
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="S5:AE5"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="G5:P5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="H6:H7"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C19:C20"/>
@@ -2919,24 +2891,25 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="G5:P5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="S5:AE5"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="AB9:AC9"/>
+    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="AB11:AC11"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2973,43 +2946,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="71"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="50"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="97"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="81"/>
     </row>
     <row r="6" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -3022,44 +2995,44 @@
         <v>36</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="51" t="s">
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="49" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="90">
+      <c r="B7" s="89">
         <v>1</v>
       </c>
-      <c r="C7" s="100" t="s">
+      <c r="C7" s="98" t="s">
         <v>90</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="39"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="13" t="s">
         <v>62</v>
       </c>
@@ -3078,289 +3051,289 @@
       <c r="O7" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="P7" s="51" t="s">
+      <c r="P7" s="49" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="91"/>
-      <c r="C8" s="101"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="99"/>
       <c r="D8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="65">
+      <c r="F8" s="63">
         <v>1</v>
       </c>
-      <c r="G8" s="65">
+      <c r="G8" s="63">
         <v>3</v>
       </c>
-      <c r="H8" s="65" t="s">
+      <c r="H8" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="21">
+      <c r="K8" s="19">
         <v>1</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="19">
         <v>1</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="19">
         <v>0</v>
       </c>
-      <c r="N8" s="21">
+      <c r="N8" s="19">
         <v>10</v>
       </c>
-      <c r="O8" s="67" t="s">
+      <c r="O8" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="P8" s="56" t="s">
+      <c r="P8" s="54" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="91"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="64" t="s">
+      <c r="B9" s="90"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="65">
+      <c r="F9" s="63">
         <v>2</v>
       </c>
-      <c r="G9" s="65">
+      <c r="G9" s="63">
         <v>1</v>
       </c>
-      <c r="H9" s="65" t="s">
+      <c r="H9" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="21">
+      <c r="K9" s="19">
         <v>1</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="19">
         <v>1</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="19">
         <v>0</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="19">
         <v>10</v>
       </c>
-      <c r="O9" s="67" t="s">
+      <c r="O9" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="P9" s="56" t="s">
+      <c r="P9" s="54" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="91"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="64" t="s">
+      <c r="B10" s="90"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="65">
+      <c r="F10" s="63">
         <v>3</v>
       </c>
-      <c r="G10" s="65">
+      <c r="G10" s="63">
         <v>8</v>
       </c>
-      <c r="H10" s="65" t="s">
+      <c r="H10" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="K10" s="21">
+      <c r="K10" s="19">
         <v>1</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="19">
         <v>0</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="19">
         <v>0</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="19">
         <v>10</v>
       </c>
-      <c r="O10" s="67" t="s">
+      <c r="O10" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="P10" s="56" t="s">
+      <c r="P10" s="54" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="91"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="64" t="s">
+      <c r="B11" s="90"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="65">
+      <c r="F11" s="63">
         <v>4</v>
       </c>
-      <c r="G11" s="65">
+      <c r="G11" s="63">
         <v>7</v>
       </c>
-      <c r="H11" s="65" t="s">
+      <c r="H11" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="K11" s="21">
+      <c r="K11" s="19">
         <v>1</v>
       </c>
-      <c r="L11" s="21">
+      <c r="L11" s="19">
         <v>-1</v>
       </c>
-      <c r="M11" s="21">
+      <c r="M11" s="19">
         <v>0</v>
       </c>
-      <c r="N11" s="21">
+      <c r="N11" s="19">
         <v>10</v>
       </c>
-      <c r="O11" s="67" t="s">
+      <c r="O11" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="P11" s="56" t="s">
+      <c r="P11" s="54" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="93"/>
-      <c r="C12" s="102"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="100"/>
       <c r="D12" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F12" s="65">
+      <c r="F12" s="63">
         <v>5</v>
       </c>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="67"/>
-      <c r="P12" s="56"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="65"/>
+      <c r="P12" s="54"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="90">
+      <c r="B13" s="89">
         <v>2</v>
       </c>
-      <c r="C13" s="90" t="s">
+      <c r="C13" s="89" t="s">
         <v>83</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F13" s="65">
+      <c r="F13" s="63">
         <v>6</v>
       </c>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="63"/>
-      <c r="P13" s="56"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="54"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="91"/>
-      <c r="C14" s="91"/>
-      <c r="D14" s="64" t="s">
+      <c r="B14" s="90"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="65">
+      <c r="F14" s="63">
         <v>7</v>
       </c>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="66"/>
-      <c r="P14" s="56"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="64"/>
+      <c r="P14" s="54"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="91"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="64" t="s">
+      <c r="B15" s="90"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="F15" s="65">
+      <c r="F15" s="63">
         <v>8</v>
       </c>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="63"/>
-      <c r="P15" s="56"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="54"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="91"/>
-      <c r="C16" s="91"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="90"/>
       <c r="D16" s="2"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="63"/>
-      <c r="P16" s="56"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="54"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="91"/>
-      <c r="C17" s="91"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="90"/>
       <c r="D17" s="2"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="63"/>
-      <c r="P17" s="56"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="61"/>
+      <c r="P17" s="54"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="92"/>
       <c r="D18" s="2"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
@@ -3371,14 +3344,14 @@
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="55"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="53"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="90">
+      <c r="B19" s="89">
         <v>3</v>
       </c>
-      <c r="C19" s="100"/>
+      <c r="C19" s="98"/>
       <c r="D19" s="2"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
@@ -3389,64 +3362,64 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="55"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="53"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="91"/>
-      <c r="C20" s="101"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="99"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="91"/>
-      <c r="C21" s="101"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="99"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="91"/>
-      <c r="C22" s="101"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="99"/>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="91"/>
-      <c r="C23" s="101"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="99"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="93"/>
-      <c r="C24" s="102"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="100"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="90">
+      <c r="B25" s="89">
         <v>4</v>
       </c>
-      <c r="C25" s="100"/>
+      <c r="C25" s="98"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="91"/>
-      <c r="C26" s="101"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="99"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="91"/>
-      <c r="C27" s="101"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="99"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="91"/>
-      <c r="C28" s="101"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="99"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="91"/>
-      <c r="C29" s="101"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="99"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="93"/>
-      <c r="C30" s="102"/>
+      <c r="B30" s="92"/>
+      <c r="C30" s="100"/>
       <c r="D30" s="2" t="s">
         <v>33</v>
       </c>
@@ -3476,10 +3449,10 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B1:P36"/>
+  <dimension ref="B1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3495,65 +3468,65 @@
     <col min="15" max="15" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="69" t="s">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="71"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="132" t="s">
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="111" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
-      <c r="K3" s="132"/>
-      <c r="L3" s="132"/>
-      <c r="M3" s="132"/>
-      <c r="N3" s="132"/>
-      <c r="O3" s="132"/>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="115" t="s">
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="111"/>
+      <c r="N3" s="111"/>
+      <c r="O3" s="111"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="130" t="s">
+      <c r="C4" s="109" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="117" t="s">
+      <c r="D4" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="128" t="s">
+      <c r="E4" s="107" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="133" t="s">
+      <c r="F4" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="134"/>
-      <c r="H4" s="134"/>
-      <c r="I4" s="134"/>
-      <c r="J4" s="134"/>
-      <c r="K4" s="134"/>
-      <c r="L4" s="134"/>
-      <c r="M4" s="135"/>
-      <c r="N4" s="82" t="s">
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="104"/>
+      <c r="N4" s="86" t="s">
         <v>68</v>
       </c>
-      <c r="O4" s="83"/>
-    </row>
-    <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="116"/>
-      <c r="C5" s="131"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="129"/>
+      <c r="O4" s="88"/>
+    </row>
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="114"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="108"/>
       <c r="F5" s="13" t="s">
         <v>62</v>
       </c>
@@ -3569,570 +3542,465 @@
       <c r="J5" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="K5" s="82" t="s">
+      <c r="K5" s="86" t="s">
         <v>67</v>
       </c>
       <c r="L5" s="87"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="51" t="s">
+      <c r="M5" s="88"/>
+      <c r="N5" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="O5" s="57" t="s">
+      <c r="O5" s="55" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14">
         <v>1</v>
       </c>
-      <c r="C6" s="113" t="s">
+      <c r="C6" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="18"/>
+      <c r="D6" s="17">
+        <v>2</v>
+      </c>
       <c r="E6" s="14">
         <v>1</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="134" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="19">
         <v>1</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="19">
         <v>1</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="19">
         <v>0</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="19">
         <v>10</v>
       </c>
-      <c r="K6" s="80" t="s">
+      <c r="K6" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="L6" s="104"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="56" t="s">
+      <c r="L6" s="133"/>
+      <c r="M6" s="96"/>
+      <c r="N6" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="O6" s="56" t="s">
+      <c r="O6" s="54" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="8">
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="19"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="18" t="s">
+        <v>104</v>
+      </c>
       <c r="E7" s="8">
         <v>3</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="134" t="s">
         <v>102</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="19">
         <v>1</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="19">
         <v>1</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="19">
         <v>0</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="19">
         <v>10</v>
       </c>
-      <c r="K7" s="80" t="s">
+      <c r="K7" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="L7" s="104"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="56" t="s">
+      <c r="L7" s="133"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="O7" s="56" t="s">
+      <c r="O7" s="54" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="8">
-        <f t="shared" ref="B8:B13" si="0">B7+1</f>
+        <f t="shared" ref="B8:B9" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="113"/>
-      <c r="D8" s="19"/>
+      <c r="C8" s="112"/>
+      <c r="D8" s="18">
+        <v>4</v>
+      </c>
       <c r="E8" s="8">
         <v>8</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="19">
         <v>1</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="19">
         <v>0</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="19">
         <v>0</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="19">
         <v>10</v>
       </c>
-      <c r="K8" s="80" t="s">
+      <c r="K8" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="L8" s="104"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="56" t="s">
+      <c r="L8" s="133"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="O8" s="56" t="s">
+      <c r="O8" s="54" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="113"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="18">
+        <v>1</v>
+      </c>
       <c r="E9" s="8">
         <v>9</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="19">
         <v>1</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="19">
         <v>1</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="19">
         <v>0</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="19">
         <v>10</v>
       </c>
-      <c r="K9" s="80" t="s">
+      <c r="K9" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="L9" s="104"/>
-      <c r="M9" s="81"/>
-      <c r="N9" s="56" t="s">
+      <c r="L9" s="133"/>
+      <c r="M9" s="96"/>
+      <c r="N9" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="O9" s="56" t="s">
+      <c r="O9" s="54" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="8">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="113"/>
-      <c r="D10" s="19">
+      <c r="C10" s="112"/>
+      <c r="D10" s="18">
+        <v>3</v>
+      </c>
+      <c r="E10" s="8">
+        <v>7</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="19">
         <v>1</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="21">
-        <v>1</v>
-      </c>
-      <c r="H10" s="21">
-        <v>1</v>
-      </c>
-      <c r="I10" s="21">
+      <c r="H10" s="19">
+        <v>-1</v>
+      </c>
+      <c r="I10" s="19">
         <v>0</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="19">
         <v>10</v>
       </c>
-      <c r="K10" s="80" t="s">
+      <c r="K10" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="L10" s="104"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="56" t="s">
+      <c r="L10" s="133"/>
+      <c r="M10" s="96"/>
+      <c r="N10" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="O10" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="O10" s="56" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C11" s="113"/>
-      <c r="D11" s="19">
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+    </row>
+    <row r="12" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="105"/>
+      <c r="L12" s="105"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="122" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="123"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="122" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="125"/>
+      <c r="J14" s="123"/>
+      <c r="K14" s="123"/>
+      <c r="L14" s="124"/>
+      <c r="M14" s="122" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" s="125"/>
+      <c r="O14" s="123"/>
+      <c r="P14" s="124"/>
+    </row>
+    <row r="15" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="119" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="120" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="106" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="106" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="121" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="130" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="126" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="127"/>
+      <c r="J15" s="106" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" s="106" t="s">
+        <v>55</v>
+      </c>
+      <c r="L15" s="121" t="s">
+        <v>56</v>
+      </c>
+      <c r="M15" s="131" t="s">
+        <v>59</v>
+      </c>
+      <c r="N15" s="106" t="s">
+        <v>54</v>
+      </c>
+      <c r="O15" s="106" t="s">
+        <v>55</v>
+      </c>
+      <c r="P15" s="121" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="119"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="106"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="130"/>
+      <c r="H16" s="128"/>
+      <c r="I16" s="129"/>
+      <c r="J16" s="106"/>
+      <c r="K16" s="106"/>
+      <c r="L16" s="121"/>
+      <c r="M16" s="132"/>
+      <c r="N16" s="106"/>
+      <c r="O16" s="106"/>
+      <c r="P16" s="121"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="22">
+        <v>5</v>
+      </c>
+      <c r="D17" s="24">
+        <v>3</v>
+      </c>
+      <c r="E17" s="24">
         <v>2</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="21">
-        <v>1</v>
-      </c>
-      <c r="H11" s="21">
-        <v>1</v>
-      </c>
-      <c r="I11" s="21">
+      <c r="F17" s="25">
+        <v>2</v>
+      </c>
+      <c r="G17" s="28">
+        <v>2</v>
+      </c>
+      <c r="H17" s="117" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="118"/>
+      <c r="J17" s="2">
+        <v>5</v>
+      </c>
+      <c r="K17" s="24">
+        <v>5</v>
+      </c>
+      <c r="L17" s="25">
         <v>0</v>
       </c>
-      <c r="J11" s="21">
-        <v>10</v>
-      </c>
-      <c r="K11" s="80" t="s">
-        <v>89</v>
-      </c>
-      <c r="L11" s="104"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="O11" s="56" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C12" s="113"/>
-      <c r="D12" s="19">
-        <v>3</v>
-      </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" s="21">
-        <v>1</v>
-      </c>
-      <c r="H12" s="21">
-        <v>-1</v>
-      </c>
-      <c r="I12" s="21">
+      <c r="M17" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="N17" s="2">
+        <v>5</v>
+      </c>
+      <c r="O17" s="24">
+        <v>5</v>
+      </c>
+      <c r="P17" s="25">
         <v>0</v>
       </c>
-      <c r="J12" s="21">
-        <v>10</v>
-      </c>
-      <c r="K12" s="80" t="s">
-        <v>89</v>
-      </c>
-      <c r="L12" s="104"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="O12" s="56" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="15">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C13" s="114"/>
-      <c r="D13" s="20">
-        <v>4</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" s="21">
-        <v>1</v>
-      </c>
-      <c r="H13" s="21">
-        <v>0</v>
-      </c>
-      <c r="I13" s="21">
-        <v>0</v>
-      </c>
-      <c r="J13" s="21">
-        <v>10</v>
-      </c>
-      <c r="K13" s="80" t="s">
-        <v>89</v>
-      </c>
-      <c r="L13" s="104"/>
-      <c r="M13" s="81"/>
-      <c r="N13" s="56" t="s">
-        <v>103</v>
-      </c>
-      <c r="O13" s="56" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-    </row>
-    <row r="15" spans="2:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="136"/>
-      <c r="L15" s="136"/>
-      <c r="M15" s="5"/>
-    </row>
-    <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M16" s="5"/>
-    </row>
-    <row r="17" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="107" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="109"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="110"/>
-      <c r="G17" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="107" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="108"/>
-      <c r="J17" s="109"/>
-      <c r="K17" s="109"/>
-      <c r="L17" s="110"/>
-      <c r="M17" s="107" t="s">
-        <v>53</v>
-      </c>
-      <c r="N17" s="108"/>
-      <c r="O17" s="109"/>
-      <c r="P17" s="110"/>
-    </row>
-    <row r="18" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="121" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="122" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="105" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="105" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="106" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="127" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" s="123" t="s">
-        <v>59</v>
-      </c>
-      <c r="I18" s="124"/>
-      <c r="J18" s="105" t="s">
-        <v>54</v>
-      </c>
-      <c r="K18" s="105" t="s">
-        <v>55</v>
-      </c>
-      <c r="L18" s="106" t="s">
-        <v>56</v>
-      </c>
-      <c r="M18" s="111" t="s">
-        <v>59</v>
-      </c>
-      <c r="N18" s="105" t="s">
-        <v>54</v>
-      </c>
-      <c r="O18" s="105" t="s">
-        <v>55</v>
-      </c>
-      <c r="P18" s="106" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="121"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="105"/>
-      <c r="E19" s="105"/>
-      <c r="F19" s="106"/>
-      <c r="G19" s="127"/>
-      <c r="H19" s="125"/>
-      <c r="I19" s="126"/>
-      <c r="J19" s="105"/>
-      <c r="K19" s="105"/>
-      <c r="L19" s="106"/>
-      <c r="M19" s="112"/>
-      <c r="N19" s="105"/>
-      <c r="O19" s="105"/>
-      <c r="P19" s="106"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="24">
-        <v>8</v>
-      </c>
-      <c r="D20" s="26">
-        <v>4</v>
-      </c>
-      <c r="E20" s="26">
-        <v>4</v>
-      </c>
-      <c r="F20" s="27">
-        <v>4</v>
-      </c>
-      <c r="G20" s="30">
-        <v>4</v>
-      </c>
-      <c r="H20" s="119" t="s">
-        <v>73</v>
-      </c>
-      <c r="I20" s="120"/>
-      <c r="J20" s="2">
-        <v>4</v>
-      </c>
-      <c r="K20" s="26">
-        <v>4</v>
-      </c>
-      <c r="L20" s="27">
-        <v>0</v>
-      </c>
-      <c r="M20" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="N20" s="2">
-        <v>8</v>
-      </c>
-      <c r="O20" s="26">
-        <v>8</v>
-      </c>
-      <c r="P20" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="M21" s="3"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M18" s="3"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="71"/>
+      <c r="M30" s="72"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="53"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="71"/>
+      <c r="M31" s="72"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="53"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="72"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="53"/>
     </row>
     <row r="33" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="75"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="72"/>
       <c r="N33" s="11"/>
-      <c r="O33" s="55"/>
-    </row>
-    <row r="34" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="74"/>
-      <c r="M34" s="75"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="55"/>
-    </row>
-    <row r="35" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="74"/>
-      <c r="M35" s="75"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="55"/>
-    </row>
-    <row r="36" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="74"/>
-      <c r="M36" s="75"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="55"/>
+      <c r="O33" s="53"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="F4:M4"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="J18:J19"/>
+  <mergeCells count="38">
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="M14:P14"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="H15:I16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B3:O3"/>
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="H18:I19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="F4:M4"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K10:M10"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="K8:M8"/>
     <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
   </mergeCells>
   <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4142,21 +4010,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5F472198D7887469049920058585067" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e76e8f6ca957e849a493f1baa4f4bb7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c46c0853-0d59-45c6-b517-3e25eac8cdf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ddeb00cc2097713d6f56fe4f26be38f" ns2:_="">
     <xsd:import namespace="c46c0853-0d59-45c6-b517-3e25eac8cdf1"/>
@@ -4300,10 +4153,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153A5999-B236-48B1-944C-C5EB94545735}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c46c0853-0d59-45c6-b517-3e25eac8cdf1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4325,19 +4203,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153A5999-B236-48B1-944C-C5EB94545735}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c46c0853-0d59-45c6-b517-3e25eac8cdf1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>